<commit_message>
📊 Update NAIC content history - 2025-10-02
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm20-table-h-i-long-term-spreads.xlsx
+++ b/docs/content_history/pbr-2025-vm20-table-h-i-long-term-spreads.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22F4616-5498-4C0C-B971-190BC46CD704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C64742A-4FA0-4FF3-9392-FEF9EC8E2DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="June_2025" sheetId="27" r:id="rId1"/>
-    <sheet name="March_2025" sheetId="26" r:id="rId2"/>
-    <sheet name="December_2024" sheetId="25" r:id="rId3"/>
-    <sheet name="LEGAL DISCLAIMER" sheetId="4" r:id="rId4"/>
+    <sheet name="September_2025" sheetId="28" r:id="rId1"/>
+    <sheet name="June_2025" sheetId="27" r:id="rId2"/>
+    <sheet name="March_2025" sheetId="26" r:id="rId3"/>
+    <sheet name="December_2024" sheetId="25" r:id="rId4"/>
+    <sheet name="LEGAL DISCLAIMER" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t>WAL</t>
   </si>
@@ -129,6 +130,12 @@
   </si>
   <si>
     <t>Table I (6/30/2025) Below Investment Grade Long Term Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table H (9/30/2025) Investment Grade Long Term Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table I (9/30/2025) Below Investment Grade Long Term Benchmark Spreads (in bps)</t>
   </si>
 </sst>
 </file>
@@ -329,7 +336,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -650,19 +657,2344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D1968-5793-4D21-B24C-89D80D0D7CAC}">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="M2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11">
+        <v>8</v>
+      </c>
+      <c r="J3" s="11">
+        <v>9</v>
+      </c>
+      <c r="K3" s="11">
+        <v>10</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11">
+        <v>11</v>
+      </c>
+      <c r="O3" s="11">
+        <v>12</v>
+      </c>
+      <c r="P3" s="11">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>14</v>
+      </c>
+      <c r="R3" s="11">
+        <v>15</v>
+      </c>
+      <c r="S3" s="11">
+        <v>16</v>
+      </c>
+      <c r="T3" s="11">
+        <v>17</v>
+      </c>
+      <c r="U3" s="11">
+        <v>18</v>
+      </c>
+      <c r="V3" s="11">
+        <v>19</v>
+      </c>
+      <c r="W3" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>21.05</v>
+      </c>
+      <c r="C5" s="2">
+        <v>28.93</v>
+      </c>
+      <c r="D5" s="2">
+        <v>36.82</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43.81</v>
+      </c>
+      <c r="F5" s="2">
+        <v>50.81</v>
+      </c>
+      <c r="G5" s="2">
+        <v>57.81</v>
+      </c>
+      <c r="H5" s="2">
+        <v>72.2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>86.59</v>
+      </c>
+      <c r="J5" s="2">
+        <v>100.98</v>
+      </c>
+      <c r="K5" s="3">
+        <v>176.46</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O5" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P5" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R5" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S5" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T5" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U5" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2">
+        <v>35.78</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44.57</v>
+      </c>
+      <c r="E6" s="2">
+        <v>52.37</v>
+      </c>
+      <c r="F6" s="2">
+        <v>60.17</v>
+      </c>
+      <c r="G6" s="2">
+        <v>67.97</v>
+      </c>
+      <c r="H6" s="2">
+        <v>83.38</v>
+      </c>
+      <c r="I6" s="2">
+        <v>98.8</v>
+      </c>
+      <c r="J6" s="2">
+        <v>114.21</v>
+      </c>
+      <c r="K6" s="3">
+        <v>183.07</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O6" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P6" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R6" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S6" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T6" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U6" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V6" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="C7" s="2">
+        <v>42.64</v>
+      </c>
+      <c r="D7" s="2">
+        <v>52.32</v>
+      </c>
+      <c r="E7" s="2">
+        <v>60.93</v>
+      </c>
+      <c r="F7" s="2">
+        <v>69.53</v>
+      </c>
+      <c r="G7" s="2">
+        <v>78.13</v>
+      </c>
+      <c r="H7" s="2">
+        <v>94.57</v>
+      </c>
+      <c r="I7" s="2">
+        <v>111.01</v>
+      </c>
+      <c r="J7" s="2">
+        <v>127.45</v>
+      </c>
+      <c r="K7" s="3">
+        <v>189.69</v>
+      </c>
+      <c r="M7" s="1">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O7" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P7" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R7" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S7" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T7" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U7" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>38.9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>49.49</v>
+      </c>
+      <c r="D8" s="2">
+        <v>60.08</v>
+      </c>
+      <c r="E8" s="2">
+        <v>69.48</v>
+      </c>
+      <c r="F8" s="2">
+        <v>78.89</v>
+      </c>
+      <c r="G8" s="2">
+        <v>88.29</v>
+      </c>
+      <c r="H8" s="2">
+        <v>105.76</v>
+      </c>
+      <c r="I8" s="2">
+        <v>123.22</v>
+      </c>
+      <c r="J8" s="2">
+        <v>140.68</v>
+      </c>
+      <c r="K8" s="3">
+        <v>196.31</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O8" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P8" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R8" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S8" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T8" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U8" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V8" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W8" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44.11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>55.1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>66.08</v>
+      </c>
+      <c r="E9" s="2">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="F9" s="2">
+        <v>86.22</v>
+      </c>
+      <c r="G9" s="2">
+        <v>96.29</v>
+      </c>
+      <c r="H9" s="2">
+        <v>114.97</v>
+      </c>
+      <c r="I9" s="2">
+        <v>133.63999999999999</v>
+      </c>
+      <c r="J9" s="2">
+        <v>152.32</v>
+      </c>
+      <c r="K9" s="3">
+        <v>202.13</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O9" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P9" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R9" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S9" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T9" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U9" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V9" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>49.32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>60.71</v>
+      </c>
+      <c r="D10" s="2">
+        <v>72.09</v>
+      </c>
+      <c r="E10" s="2">
+        <v>82.82</v>
+      </c>
+      <c r="F10" s="2">
+        <v>93.55</v>
+      </c>
+      <c r="G10" s="2">
+        <v>104.28</v>
+      </c>
+      <c r="H10" s="2">
+        <v>124.17</v>
+      </c>
+      <c r="I10" s="2">
+        <v>144.06</v>
+      </c>
+      <c r="J10" s="2">
+        <v>163.95</v>
+      </c>
+      <c r="K10" s="3">
+        <v>207.94</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6</v>
+      </c>
+      <c r="N10" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O10" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P10" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R10" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S10" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T10" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U10" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>54.98</v>
+      </c>
+      <c r="C11" s="2">
+        <v>65.95</v>
+      </c>
+      <c r="D11" s="2">
+        <v>76.930000000000007</v>
+      </c>
+      <c r="E11" s="2">
+        <v>87.63</v>
+      </c>
+      <c r="F11" s="2">
+        <v>98.33</v>
+      </c>
+      <c r="G11" s="2">
+        <v>109.02</v>
+      </c>
+      <c r="H11" s="2">
+        <v>129.03</v>
+      </c>
+      <c r="I11" s="2">
+        <v>149.03</v>
+      </c>
+      <c r="J11" s="2">
+        <v>169.04</v>
+      </c>
+      <c r="K11" s="3">
+        <v>210.48</v>
+      </c>
+      <c r="M11" s="1">
+        <v>7</v>
+      </c>
+      <c r="N11" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O11" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P11" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R11" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S11" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T11" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U11" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V11" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W11" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>60.63</v>
+      </c>
+      <c r="C12" s="2">
+        <v>71.2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>81.77</v>
+      </c>
+      <c r="E12" s="2">
+        <v>92.43</v>
+      </c>
+      <c r="F12" s="2">
+        <v>103.1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>113.76</v>
+      </c>
+      <c r="H12" s="2">
+        <v>133.88</v>
+      </c>
+      <c r="I12" s="2">
+        <v>154</v>
+      </c>
+      <c r="J12" s="2">
+        <v>174.12</v>
+      </c>
+      <c r="K12" s="3">
+        <v>213.03</v>
+      </c>
+      <c r="M12" s="1">
+        <v>8</v>
+      </c>
+      <c r="N12" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O12" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P12" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R12" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S12" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T12" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U12" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V12" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>66.290000000000006</v>
+      </c>
+      <c r="C13" s="2">
+        <v>76.45</v>
+      </c>
+      <c r="D13" s="2">
+        <v>86.61</v>
+      </c>
+      <c r="E13" s="2">
+        <v>97.24</v>
+      </c>
+      <c r="F13" s="2">
+        <v>107.87</v>
+      </c>
+      <c r="G13" s="2">
+        <v>118.5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>138.72999999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>158.96</v>
+      </c>
+      <c r="J13" s="2">
+        <v>179.2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>215.57</v>
+      </c>
+      <c r="M13" s="1">
+        <v>9</v>
+      </c>
+      <c r="N13" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O13" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P13" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R13" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S13" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T13" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U13" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V13" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W13" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <v>67.63</v>
+      </c>
+      <c r="C14" s="2">
+        <v>78.16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>88.68</v>
+      </c>
+      <c r="E14" s="2">
+        <v>99.1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>109.51</v>
+      </c>
+      <c r="G14" s="2">
+        <v>119.93</v>
+      </c>
+      <c r="H14" s="2">
+        <v>140.38</v>
+      </c>
+      <c r="I14" s="2">
+        <v>160.83000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>181.28</v>
+      </c>
+      <c r="K14" s="3">
+        <v>216.61</v>
+      </c>
+      <c r="M14" s="1">
+        <v>10</v>
+      </c>
+      <c r="N14" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O14" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P14" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R14" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S14" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T14" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U14" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V14" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W14" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>68.98</v>
+      </c>
+      <c r="C15" s="2">
+        <v>79.86</v>
+      </c>
+      <c r="D15" s="2">
+        <v>90.75</v>
+      </c>
+      <c r="E15" s="2">
+        <v>100.95</v>
+      </c>
+      <c r="F15" s="2">
+        <v>111.15</v>
+      </c>
+      <c r="G15" s="2">
+        <v>121.35</v>
+      </c>
+      <c r="H15" s="2">
+        <v>142.02000000000001</v>
+      </c>
+      <c r="I15" s="2">
+        <v>162.69</v>
+      </c>
+      <c r="J15" s="2">
+        <v>183.36</v>
+      </c>
+      <c r="K15" s="3">
+        <v>217.65</v>
+      </c>
+      <c r="M15" s="1">
+        <v>11</v>
+      </c>
+      <c r="N15" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O15" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P15" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R15" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S15" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T15" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U15" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V15" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W15" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>70.319999999999993</v>
+      </c>
+      <c r="C16" s="2">
+        <v>81.569999999999993</v>
+      </c>
+      <c r="D16" s="2">
+        <v>92.82</v>
+      </c>
+      <c r="E16" s="2">
+        <v>102.8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>112.79</v>
+      </c>
+      <c r="G16" s="2">
+        <v>122.77</v>
+      </c>
+      <c r="H16" s="2">
+        <v>143.66</v>
+      </c>
+      <c r="I16" s="2">
+        <v>164.55</v>
+      </c>
+      <c r="J16" s="2">
+        <v>185.44</v>
+      </c>
+      <c r="K16" s="3">
+        <v>218.69</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12</v>
+      </c>
+      <c r="N16" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O16" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P16" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R16" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S16" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T16" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U16" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V16" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W16" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>71.67</v>
+      </c>
+      <c r="C17" s="2">
+        <v>83.28</v>
+      </c>
+      <c r="D17" s="2">
+        <v>94.89</v>
+      </c>
+      <c r="E17" s="2">
+        <v>104.66</v>
+      </c>
+      <c r="F17" s="2">
+        <v>114.43</v>
+      </c>
+      <c r="G17" s="2">
+        <v>124.2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>145.31</v>
+      </c>
+      <c r="I17" s="2">
+        <v>166.42</v>
+      </c>
+      <c r="J17" s="2">
+        <v>187.53</v>
+      </c>
+      <c r="K17" s="3">
+        <v>219.73</v>
+      </c>
+      <c r="M17" s="1">
+        <v>13</v>
+      </c>
+      <c r="N17" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O17" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P17" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R17" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S17" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T17" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U17" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2">
+        <v>73.02</v>
+      </c>
+      <c r="C18" s="2">
+        <v>84.99</v>
+      </c>
+      <c r="D18" s="2">
+        <v>96.95</v>
+      </c>
+      <c r="E18" s="2">
+        <v>106.51</v>
+      </c>
+      <c r="F18" s="2">
+        <v>116.07</v>
+      </c>
+      <c r="G18" s="2">
+        <v>125.62</v>
+      </c>
+      <c r="H18" s="2">
+        <v>146.94999999999999</v>
+      </c>
+      <c r="I18" s="2">
+        <v>168.28</v>
+      </c>
+      <c r="J18" s="2">
+        <v>189.61</v>
+      </c>
+      <c r="K18" s="3">
+        <v>220.77</v>
+      </c>
+      <c r="M18" s="1">
+        <v>14</v>
+      </c>
+      <c r="N18" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O18" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P18" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R18" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S18" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T18" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U18" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W18" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2">
+        <v>74.36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>86.69</v>
+      </c>
+      <c r="D19" s="2">
+        <v>99.02</v>
+      </c>
+      <c r="E19" s="2">
+        <v>108.37</v>
+      </c>
+      <c r="F19" s="2">
+        <v>117.71</v>
+      </c>
+      <c r="G19" s="2">
+        <v>127.05</v>
+      </c>
+      <c r="H19" s="2">
+        <v>148.6</v>
+      </c>
+      <c r="I19" s="2">
+        <v>170.14</v>
+      </c>
+      <c r="J19" s="2">
+        <v>191.69</v>
+      </c>
+      <c r="K19" s="3">
+        <v>221.81</v>
+      </c>
+      <c r="M19" s="1">
+        <v>15</v>
+      </c>
+      <c r="N19" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O19" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P19" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R19" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S19" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T19" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U19" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V19" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W19" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2">
+        <v>75.709999999999994</v>
+      </c>
+      <c r="C20" s="2">
+        <v>88.4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>101.09</v>
+      </c>
+      <c r="E20" s="2">
+        <v>110.22</v>
+      </c>
+      <c r="F20" s="2">
+        <v>119.35</v>
+      </c>
+      <c r="G20" s="2">
+        <v>128.47</v>
+      </c>
+      <c r="H20" s="2">
+        <v>150.24</v>
+      </c>
+      <c r="I20" s="2">
+        <v>172.01</v>
+      </c>
+      <c r="J20" s="2">
+        <v>193.77</v>
+      </c>
+      <c r="K20" s="3">
+        <v>222.85</v>
+      </c>
+      <c r="M20" s="1">
+        <v>16</v>
+      </c>
+      <c r="N20" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O20" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P20" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R20" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S20" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T20" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U20" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2">
+        <v>77.05</v>
+      </c>
+      <c r="C21" s="2">
+        <v>90.11</v>
+      </c>
+      <c r="D21" s="2">
+        <v>103.16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>112.07</v>
+      </c>
+      <c r="F21" s="2">
+        <v>120.99</v>
+      </c>
+      <c r="G21" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="H21" s="2">
+        <v>151.88</v>
+      </c>
+      <c r="I21" s="2">
+        <v>173.87</v>
+      </c>
+      <c r="J21" s="2">
+        <v>195.86</v>
+      </c>
+      <c r="K21" s="3">
+        <v>223.9</v>
+      </c>
+      <c r="M21" s="1">
+        <v>17</v>
+      </c>
+      <c r="N21" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O21" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P21" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R21" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S21" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T21" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U21" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V21" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W21" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C22" s="2">
+        <v>91.81</v>
+      </c>
+      <c r="D22" s="2">
+        <v>105.23</v>
+      </c>
+      <c r="E22" s="2">
+        <v>113.93</v>
+      </c>
+      <c r="F22" s="2">
+        <v>122.63</v>
+      </c>
+      <c r="G22" s="2">
+        <v>131.32</v>
+      </c>
+      <c r="H22" s="2">
+        <v>153.53</v>
+      </c>
+      <c r="I22" s="2">
+        <v>175.73</v>
+      </c>
+      <c r="J22" s="2">
+        <v>197.94</v>
+      </c>
+      <c r="K22" s="3">
+        <v>224.94</v>
+      </c>
+      <c r="M22" s="1">
+        <v>18</v>
+      </c>
+      <c r="N22" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O22" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P22" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R22" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S22" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T22" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U22" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V22" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W22" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2">
+        <v>79.739999999999995</v>
+      </c>
+      <c r="C23" s="2">
+        <v>93.52</v>
+      </c>
+      <c r="D23" s="2">
+        <v>107.3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>115.78</v>
+      </c>
+      <c r="F23" s="2">
+        <v>124.26</v>
+      </c>
+      <c r="G23" s="2">
+        <v>132.75</v>
+      </c>
+      <c r="H23" s="2">
+        <v>155.16999999999999</v>
+      </c>
+      <c r="I23" s="2">
+        <v>177.6</v>
+      </c>
+      <c r="J23" s="2">
+        <v>200.02</v>
+      </c>
+      <c r="K23" s="3">
+        <v>225.98</v>
+      </c>
+      <c r="M23" s="1">
+        <v>19</v>
+      </c>
+      <c r="N23" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O23" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P23" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R23" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S23" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T23" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U23" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V23" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W23" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2">
+        <v>81.09</v>
+      </c>
+      <c r="C24" s="2">
+        <v>95.23</v>
+      </c>
+      <c r="D24" s="2">
+        <v>109.37</v>
+      </c>
+      <c r="E24" s="2">
+        <v>117.64</v>
+      </c>
+      <c r="F24" s="2">
+        <v>125.9</v>
+      </c>
+      <c r="G24" s="2">
+        <v>134.16999999999999</v>
+      </c>
+      <c r="H24" s="2">
+        <v>156.82</v>
+      </c>
+      <c r="I24" s="2">
+        <v>179.46</v>
+      </c>
+      <c r="J24" s="2">
+        <v>202.1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>227.02</v>
+      </c>
+      <c r="M24" s="1">
+        <v>20</v>
+      </c>
+      <c r="N24" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O24" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P24" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R24" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S24" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T24" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U24" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V24" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W24" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2">
+        <v>82.44</v>
+      </c>
+      <c r="C25" s="2">
+        <v>96.94</v>
+      </c>
+      <c r="D25" s="2">
+        <v>111.44</v>
+      </c>
+      <c r="E25" s="2">
+        <v>119.49</v>
+      </c>
+      <c r="F25" s="2">
+        <v>127.54</v>
+      </c>
+      <c r="G25" s="2">
+        <v>135.6</v>
+      </c>
+      <c r="H25" s="2">
+        <v>158.46</v>
+      </c>
+      <c r="I25" s="2">
+        <v>181.32</v>
+      </c>
+      <c r="J25" s="2">
+        <v>204.19</v>
+      </c>
+      <c r="K25" s="3">
+        <v>228.06</v>
+      </c>
+      <c r="M25" s="1">
+        <v>21</v>
+      </c>
+      <c r="N25" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O25" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P25" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R25" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S25" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T25" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U25" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V25" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W25" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2">
+        <v>83.78</v>
+      </c>
+      <c r="C26" s="2">
+        <v>98.64</v>
+      </c>
+      <c r="D26" s="2">
+        <v>113.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>121.34</v>
+      </c>
+      <c r="F26" s="2">
+        <v>129.18</v>
+      </c>
+      <c r="G26" s="2">
+        <v>137.02000000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <v>160.11000000000001</v>
+      </c>
+      <c r="I26" s="2">
+        <v>183.19</v>
+      </c>
+      <c r="J26" s="2">
+        <v>206.27</v>
+      </c>
+      <c r="K26" s="3">
+        <v>229.1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>22</v>
+      </c>
+      <c r="N26" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O26" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P26" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R26" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S26" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T26" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U26" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V26" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W26" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2">
+        <v>85.13</v>
+      </c>
+      <c r="C27" s="2">
+        <v>100.35</v>
+      </c>
+      <c r="D27" s="2">
+        <v>115.57</v>
+      </c>
+      <c r="E27" s="2">
+        <v>123.2</v>
+      </c>
+      <c r="F27" s="2">
+        <v>130.82</v>
+      </c>
+      <c r="G27" s="2">
+        <v>138.44999999999999</v>
+      </c>
+      <c r="H27" s="2">
+        <v>161.75</v>
+      </c>
+      <c r="I27" s="2">
+        <v>185.05</v>
+      </c>
+      <c r="J27" s="2">
+        <v>208.35</v>
+      </c>
+      <c r="K27" s="3">
+        <v>230.14</v>
+      </c>
+      <c r="M27" s="1">
+        <v>23</v>
+      </c>
+      <c r="N27" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O27" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P27" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R27" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S27" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T27" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U27" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V27" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2">
+        <v>86.47</v>
+      </c>
+      <c r="C28" s="2">
+        <v>102.06</v>
+      </c>
+      <c r="D28" s="2">
+        <v>117.64</v>
+      </c>
+      <c r="E28" s="2">
+        <v>125.05</v>
+      </c>
+      <c r="F28" s="2">
+        <v>132.46</v>
+      </c>
+      <c r="G28" s="2">
+        <v>139.87</v>
+      </c>
+      <c r="H28" s="2">
+        <v>163.38999999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>186.91</v>
+      </c>
+      <c r="J28" s="2">
+        <v>210.44</v>
+      </c>
+      <c r="K28" s="3">
+        <v>231.18</v>
+      </c>
+      <c r="M28" s="1">
+        <v>24</v>
+      </c>
+      <c r="N28" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O28" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P28" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R28" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S28" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T28" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U28" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V28" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2">
+        <v>87.82</v>
+      </c>
+      <c r="C29" s="2">
+        <v>103.76</v>
+      </c>
+      <c r="D29" s="2">
+        <v>119.71</v>
+      </c>
+      <c r="E29" s="2">
+        <v>126.91</v>
+      </c>
+      <c r="F29" s="2">
+        <v>134.1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>165.04</v>
+      </c>
+      <c r="I29" s="2">
+        <v>188.78</v>
+      </c>
+      <c r="J29" s="2">
+        <v>212.52</v>
+      </c>
+      <c r="K29" s="3">
+        <v>232.23</v>
+      </c>
+      <c r="M29" s="1">
+        <v>25</v>
+      </c>
+      <c r="N29" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O29" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P29" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R29" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S29" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T29" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U29" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V29" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W29" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2">
+        <v>89.17</v>
+      </c>
+      <c r="C30" s="2">
+        <v>105.47</v>
+      </c>
+      <c r="D30" s="2">
+        <v>121.78</v>
+      </c>
+      <c r="E30" s="2">
+        <v>128.76</v>
+      </c>
+      <c r="F30" s="2">
+        <v>135.74</v>
+      </c>
+      <c r="G30" s="2">
+        <v>142.72</v>
+      </c>
+      <c r="H30" s="2">
+        <v>166.68</v>
+      </c>
+      <c r="I30" s="2">
+        <v>190.64</v>
+      </c>
+      <c r="J30" s="2">
+        <v>214.6</v>
+      </c>
+      <c r="K30" s="3">
+        <v>233.27</v>
+      </c>
+      <c r="M30" s="1">
+        <v>26</v>
+      </c>
+      <c r="N30" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O30" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P30" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R30" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S30" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T30" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U30" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V30" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2">
+        <v>90.51</v>
+      </c>
+      <c r="C31" s="2">
+        <v>107.18</v>
+      </c>
+      <c r="D31" s="2">
+        <v>123.85</v>
+      </c>
+      <c r="E31" s="2">
+        <v>130.61000000000001</v>
+      </c>
+      <c r="F31" s="2">
+        <v>137.38</v>
+      </c>
+      <c r="G31" s="2">
+        <v>144.15</v>
+      </c>
+      <c r="H31" s="2">
+        <v>168.33</v>
+      </c>
+      <c r="I31" s="2">
+        <v>192.5</v>
+      </c>
+      <c r="J31" s="2">
+        <v>216.68</v>
+      </c>
+      <c r="K31" s="3">
+        <v>234.31</v>
+      </c>
+      <c r="M31" s="1">
+        <v>27</v>
+      </c>
+      <c r="N31" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O31" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P31" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R31" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S31" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T31" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U31" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V31" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W31" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2">
+        <v>91.86</v>
+      </c>
+      <c r="C32" s="2">
+        <v>108.89</v>
+      </c>
+      <c r="D32" s="2">
+        <v>125.92</v>
+      </c>
+      <c r="E32" s="2">
+        <v>132.47</v>
+      </c>
+      <c r="F32" s="2">
+        <v>139.02000000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <v>145.57</v>
+      </c>
+      <c r="H32" s="2">
+        <v>169.97</v>
+      </c>
+      <c r="I32" s="2">
+        <v>194.37</v>
+      </c>
+      <c r="J32" s="2">
+        <v>218.77</v>
+      </c>
+      <c r="K32" s="3">
+        <v>235.35</v>
+      </c>
+      <c r="M32" s="1">
+        <v>28</v>
+      </c>
+      <c r="N32" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O32" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P32" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R32" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S32" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T32" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U32" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V32" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W32" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2">
+        <v>93.2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>110.59</v>
+      </c>
+      <c r="D33" s="2">
+        <v>127.98</v>
+      </c>
+      <c r="E33" s="2">
+        <v>134.32</v>
+      </c>
+      <c r="F33" s="2">
+        <v>140.66</v>
+      </c>
+      <c r="G33" s="2">
+        <v>147</v>
+      </c>
+      <c r="H33" s="2">
+        <v>171.61</v>
+      </c>
+      <c r="I33" s="2">
+        <v>196.23</v>
+      </c>
+      <c r="J33" s="2">
+        <v>220.85</v>
+      </c>
+      <c r="K33" s="3">
+        <v>236.39</v>
+      </c>
+      <c r="M33" s="1">
+        <v>29</v>
+      </c>
+      <c r="N33" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O33" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P33" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R33" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S33" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T33" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U33" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V33" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W33" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2">
+        <v>94.55</v>
+      </c>
+      <c r="C34" s="2">
+        <v>112.3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>130.05000000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>136.18</v>
+      </c>
+      <c r="F34" s="2">
+        <v>142.30000000000001</v>
+      </c>
+      <c r="G34" s="2">
+        <v>148.41999999999999</v>
+      </c>
+      <c r="H34" s="2">
+        <v>173.26</v>
+      </c>
+      <c r="I34" s="2">
+        <v>198.09</v>
+      </c>
+      <c r="J34" s="2">
+        <v>222.93</v>
+      </c>
+      <c r="K34" s="3">
+        <v>237.43</v>
+      </c>
+      <c r="M34" s="1">
+        <v>30</v>
+      </c>
+      <c r="N34" s="3">
+        <v>251.93</v>
+      </c>
+      <c r="O34" s="3">
+        <v>307.58999999999997</v>
+      </c>
+      <c r="P34" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>418.9</v>
+      </c>
+      <c r="R34" s="3">
+        <v>474.56</v>
+      </c>
+      <c r="S34" s="3">
+        <v>637.49</v>
+      </c>
+      <c r="T34" s="3">
+        <v>800.43</v>
+      </c>
+      <c r="U34" s="3">
+        <v>963.37</v>
+      </c>
+      <c r="V34" s="3">
+        <v>1126.31</v>
+      </c>
+      <c r="W34" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2">
+        <v>69.937666666666672</v>
+      </c>
+      <c r="C35" s="2">
+        <v>82.868333333333339</v>
+      </c>
+      <c r="D35" s="2">
+        <v>95.799000000000007</v>
+      </c>
+      <c r="E35" s="2">
+        <v>104.44066666666667</v>
+      </c>
+      <c r="F35" s="2">
+        <v>113.08200000000002</v>
+      </c>
+      <c r="G35" s="2">
+        <v>121.72266666666665</v>
+      </c>
+      <c r="H35" s="2">
+        <v>142.995</v>
+      </c>
+      <c r="I35" s="2">
+        <v>164.26566666666665</v>
+      </c>
+      <c r="J35" s="2">
+        <v>185.53833333333341</v>
+      </c>
+      <c r="K35" s="2">
+        <v>218.73633333333342</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="3">
+        <v>251.93000000000012</v>
+      </c>
+      <c r="O35" s="3">
+        <v>307.59000000000009</v>
+      </c>
+      <c r="P35" s="3">
+        <v>363.25</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>418.89999999999975</v>
+      </c>
+      <c r="R35" s="3">
+        <v>474.55999999999989</v>
+      </c>
+      <c r="S35" s="3">
+        <v>637.49000000000012</v>
+      </c>
+      <c r="T35" s="3">
+        <v>800.43000000000018</v>
+      </c>
+      <c r="U35" s="3">
+        <v>963.36999999999978</v>
+      </c>
+      <c r="V35" s="3">
+        <v>1126.3100000000004</v>
+      </c>
+      <c r="W35" s="3">
+        <v>1289.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="N2:W2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3790BBC8-1243-4A56-B780-75692A787EEC}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -690,7 +3022,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -722,7 +3054,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -790,7 +3122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -858,7 +3190,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -926,7 +3258,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -994,7 +3326,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1062,7 +3394,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1130,7 +3462,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1198,7 +3530,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1266,7 +3598,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1334,7 +3666,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1402,7 +3734,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1470,7 +3802,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1538,7 +3870,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1606,7 +3938,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1674,7 +4006,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1742,7 +4074,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1810,7 +4142,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1878,7 +4210,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1946,7 +4278,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2014,7 +4346,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -2082,7 +4414,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2150,7 +4482,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2218,7 +4550,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2286,7 +4618,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2354,7 +4686,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2422,7 +4754,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2490,7 +4822,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2558,7 +4890,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -2626,7 +4958,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -2694,7 +5026,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -2762,7 +5094,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2830,7 +5162,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -2898,7 +5230,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -2975,20 +5307,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FD970D-7BFD-41BD-A958-70C0FE799EAC}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -3016,7 +5348,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3048,7 +5380,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3116,7 +5448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -3184,7 +5516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3252,7 +5584,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3320,7 +5652,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3388,7 +5720,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -3456,7 +5788,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -3524,7 +5856,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -3592,7 +5924,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -3660,7 +5992,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -3728,7 +6060,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -3796,7 +6128,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -3864,7 +6196,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -3932,7 +6264,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -4000,7 +6332,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -4068,7 +6400,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -4136,7 +6468,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -4204,7 +6536,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -4272,7 +6604,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4340,7 +6672,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4408,7 +6740,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -4476,7 +6808,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -4544,7 +6876,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -4612,7 +6944,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -4680,7 +7012,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -4748,7 +7080,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -4816,7 +7148,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -4884,7 +7216,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -4952,7 +7284,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -5020,7 +7352,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -5088,7 +7420,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -5156,7 +7488,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -5224,7 +7556,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -5301,20 +7633,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91798AA-0655-457F-85E2-BCBDCB548CAE}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -5342,7 +7674,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -5374,7 +7706,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -5442,7 +7774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -5510,7 +7842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -5578,7 +7910,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -5646,7 +7978,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -5714,7 +8046,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -5782,7 +8114,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -5850,7 +8182,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -5918,7 +8250,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -5986,7 +8318,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -6054,7 +8386,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -6122,7 +8454,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -6190,7 +8522,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -6258,7 +8590,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -6326,7 +8658,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -6394,7 +8726,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -6462,7 +8794,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -6530,7 +8862,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -6598,7 +8930,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -6666,7 +8998,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -6734,7 +9066,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -6802,7 +9134,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -6870,7 +9202,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -6938,7 +9270,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -7006,7 +9338,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -7074,7 +9406,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -7142,7 +9474,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -7210,7 +9542,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -7278,7 +9610,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -7346,7 +9678,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -7414,7 +9746,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -7482,7 +9814,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -7550,7 +9882,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -7627,7 +9959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFFF00"/>
@@ -7636,7 +9968,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-03
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm20-table-h-i-long-term-spreads.xlsx
+++ b/docs/content_history/pbr-2025-vm20-table-h-i-long-term-spreads.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C64742A-4FA0-4FF3-9392-FEF9EC8E2DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D6F1CD-F77B-41EA-B737-FD8583E2159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="September_2025" sheetId="28" r:id="rId1"/>
-    <sheet name="June_2025" sheetId="27" r:id="rId2"/>
-    <sheet name="March_2025" sheetId="26" r:id="rId3"/>
-    <sheet name="December_2024" sheetId="25" r:id="rId4"/>
-    <sheet name="LEGAL DISCLAIMER" sheetId="4" r:id="rId5"/>
+    <sheet name="December_2025" sheetId="29" r:id="rId1"/>
+    <sheet name="September_2025" sheetId="28" r:id="rId2"/>
+    <sheet name="June_2025" sheetId="27" r:id="rId3"/>
+    <sheet name="March_2025" sheetId="26" r:id="rId4"/>
+    <sheet name="December_2024" sheetId="25" r:id="rId5"/>
+    <sheet name="LEGAL DISCLAIMER" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="36">
   <si>
     <t>WAL</t>
   </si>
@@ -136,6 +137,12 @@
   </si>
   <si>
     <t>Table I (9/30/2025) Below Investment Grade Long Term Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table H (12/31/2025) Investment Grade Long Term Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table I (12/31/2025) Below Investment Grade Long Term Benchmark Spreads (in bps)</t>
   </si>
 </sst>
 </file>
@@ -336,7 +343,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -657,18 +664,2345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D1968-5793-4D21-B24C-89D80D0D7CAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BF4DDD-FF0B-4F49-A7AA-1582BBDA098E}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="13" max="13" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="M2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11">
+        <v>8</v>
+      </c>
+      <c r="J3" s="11">
+        <v>9</v>
+      </c>
+      <c r="K3" s="11">
+        <v>10</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11">
+        <v>11</v>
+      </c>
+      <c r="O3" s="11">
+        <v>12</v>
+      </c>
+      <c r="P3" s="11">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>14</v>
+      </c>
+      <c r="R3" s="11">
+        <v>15</v>
+      </c>
+      <c r="S3" s="11">
+        <v>16</v>
+      </c>
+      <c r="T3" s="11">
+        <v>17</v>
+      </c>
+      <c r="U3" s="11">
+        <v>18</v>
+      </c>
+      <c r="V3" s="11">
+        <v>19</v>
+      </c>
+      <c r="W3" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20.46</v>
+      </c>
+      <c r="C5" s="2">
+        <v>28.28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>36.090000000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42.98</v>
+      </c>
+      <c r="F5" s="2">
+        <v>49.86</v>
+      </c>
+      <c r="G5" s="2">
+        <v>56.75</v>
+      </c>
+      <c r="H5" s="2">
+        <v>70.819999999999993</v>
+      </c>
+      <c r="I5" s="2">
+        <v>84.88</v>
+      </c>
+      <c r="J5" s="2">
+        <v>98.95</v>
+      </c>
+      <c r="K5" s="3">
+        <v>173.41</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O5" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P5" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R5" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S5" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T5" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U5" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>26.34</v>
+      </c>
+      <c r="C6" s="2">
+        <v>34.96</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43.58</v>
+      </c>
+      <c r="E6" s="2">
+        <v>51.26</v>
+      </c>
+      <c r="F6" s="2">
+        <v>58.94</v>
+      </c>
+      <c r="G6" s="2">
+        <v>66.62</v>
+      </c>
+      <c r="H6" s="2">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="I6" s="2">
+        <v>97.02</v>
+      </c>
+      <c r="J6" s="2">
+        <v>112.22</v>
+      </c>
+      <c r="K6" s="3">
+        <v>180.04</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O6" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P6" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R6" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S6" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T6" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U6" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V6" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>32.22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>41.64</v>
+      </c>
+      <c r="D7" s="2">
+        <v>51.06</v>
+      </c>
+      <c r="E7" s="2">
+        <v>59.54</v>
+      </c>
+      <c r="F7" s="2">
+        <v>68.010000000000005</v>
+      </c>
+      <c r="G7" s="2">
+        <v>76.489999999999995</v>
+      </c>
+      <c r="H7" s="2">
+        <v>92.82</v>
+      </c>
+      <c r="I7" s="2">
+        <v>109.15</v>
+      </c>
+      <c r="J7" s="2">
+        <v>125.48</v>
+      </c>
+      <c r="K7" s="3">
+        <v>186.67</v>
+      </c>
+      <c r="M7" s="1">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O7" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P7" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R7" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S7" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T7" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U7" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>38.11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>48.33</v>
+      </c>
+      <c r="D8" s="2">
+        <v>58.55</v>
+      </c>
+      <c r="E8" s="2">
+        <v>67.819999999999993</v>
+      </c>
+      <c r="F8" s="2">
+        <v>77.09</v>
+      </c>
+      <c r="G8" s="2">
+        <v>86.36</v>
+      </c>
+      <c r="H8" s="2">
+        <v>103.82</v>
+      </c>
+      <c r="I8" s="2">
+        <v>121.28</v>
+      </c>
+      <c r="J8" s="2">
+        <v>138.75</v>
+      </c>
+      <c r="K8" s="3">
+        <v>193.3</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O8" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P8" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R8" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S8" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T8" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U8" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V8" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W8" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>53.83</v>
+      </c>
+      <c r="D9" s="2">
+        <v>64.36</v>
+      </c>
+      <c r="E9" s="2">
+        <v>74.290000000000006</v>
+      </c>
+      <c r="F9" s="2">
+        <v>84.21</v>
+      </c>
+      <c r="G9" s="2">
+        <v>94.14</v>
+      </c>
+      <c r="H9" s="2">
+        <v>112.81</v>
+      </c>
+      <c r="I9" s="2">
+        <v>131.47999999999999</v>
+      </c>
+      <c r="J9" s="2">
+        <v>150.16</v>
+      </c>
+      <c r="K9" s="3">
+        <v>199.01</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O9" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P9" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R9" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S9" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T9" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U9" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V9" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>48.49</v>
+      </c>
+      <c r="C10" s="2">
+        <v>59.33</v>
+      </c>
+      <c r="D10" s="2">
+        <v>70.180000000000007</v>
+      </c>
+      <c r="E10" s="2">
+        <v>80.760000000000005</v>
+      </c>
+      <c r="F10" s="2">
+        <v>91.34</v>
+      </c>
+      <c r="G10" s="2">
+        <v>101.92</v>
+      </c>
+      <c r="H10" s="2">
+        <v>121.8</v>
+      </c>
+      <c r="I10" s="2">
+        <v>141.68</v>
+      </c>
+      <c r="J10" s="2">
+        <v>161.57</v>
+      </c>
+      <c r="K10" s="3">
+        <v>204.72</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6</v>
+      </c>
+      <c r="N10" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O10" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P10" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R10" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S10" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T10" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U10" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>54.22</v>
+      </c>
+      <c r="C11" s="2">
+        <v>64.69</v>
+      </c>
+      <c r="D11" s="2">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="E11" s="2">
+        <v>85.74</v>
+      </c>
+      <c r="F11" s="2">
+        <v>96.33</v>
+      </c>
+      <c r="G11" s="2">
+        <v>106.92</v>
+      </c>
+      <c r="H11" s="2">
+        <v>126.9</v>
+      </c>
+      <c r="I11" s="2">
+        <v>146.88</v>
+      </c>
+      <c r="J11" s="2">
+        <v>166.86</v>
+      </c>
+      <c r="K11" s="3">
+        <v>207.36</v>
+      </c>
+      <c r="M11" s="1">
+        <v>7</v>
+      </c>
+      <c r="N11" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O11" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P11" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R11" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S11" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T11" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U11" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V11" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W11" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>59.95</v>
+      </c>
+      <c r="C12" s="2">
+        <v>70.040000000000006</v>
+      </c>
+      <c r="D12" s="2">
+        <v>80.13</v>
+      </c>
+      <c r="E12" s="2">
+        <v>90.73</v>
+      </c>
+      <c r="F12" s="2">
+        <v>101.33</v>
+      </c>
+      <c r="G12" s="2">
+        <v>111.92</v>
+      </c>
+      <c r="H12" s="2">
+        <v>132</v>
+      </c>
+      <c r="I12" s="2">
+        <v>152.07</v>
+      </c>
+      <c r="J12" s="2">
+        <v>172.15</v>
+      </c>
+      <c r="K12" s="3">
+        <v>210.01</v>
+      </c>
+      <c r="M12" s="1">
+        <v>8</v>
+      </c>
+      <c r="N12" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O12" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P12" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R12" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S12" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T12" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U12" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V12" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>65.69</v>
+      </c>
+      <c r="C13" s="2">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D13" s="2">
+        <v>85.1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>95.71</v>
+      </c>
+      <c r="F13" s="2">
+        <v>106.32</v>
+      </c>
+      <c r="G13" s="2">
+        <v>116.93</v>
+      </c>
+      <c r="H13" s="2">
+        <v>137.1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>157.27000000000001</v>
+      </c>
+      <c r="J13" s="2">
+        <v>177.44</v>
+      </c>
+      <c r="K13" s="3">
+        <v>212.65</v>
+      </c>
+      <c r="M13" s="1">
+        <v>9</v>
+      </c>
+      <c r="N13" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O13" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P13" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R13" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S13" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T13" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U13" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V13" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W13" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <v>67.02</v>
+      </c>
+      <c r="C14" s="2">
+        <v>77.11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>87.19</v>
+      </c>
+      <c r="E14" s="2">
+        <v>97.61</v>
+      </c>
+      <c r="F14" s="2">
+        <v>108.04</v>
+      </c>
+      <c r="G14" s="2">
+        <v>118.47</v>
+      </c>
+      <c r="H14" s="2">
+        <v>138.83000000000001</v>
+      </c>
+      <c r="I14" s="2">
+        <v>159.19</v>
+      </c>
+      <c r="J14" s="2">
+        <v>179.55</v>
+      </c>
+      <c r="K14" s="3">
+        <v>213.7</v>
+      </c>
+      <c r="M14" s="1">
+        <v>10</v>
+      </c>
+      <c r="N14" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O14" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P14" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R14" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S14" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T14" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U14" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V14" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W14" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>68.36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>78.819999999999993</v>
+      </c>
+      <c r="D15" s="2">
+        <v>89.27</v>
+      </c>
+      <c r="E15" s="2">
+        <v>99.52</v>
+      </c>
+      <c r="F15" s="2">
+        <v>109.76</v>
+      </c>
+      <c r="G15" s="2">
+        <v>120.01</v>
+      </c>
+      <c r="H15" s="2">
+        <v>140.56</v>
+      </c>
+      <c r="I15" s="2">
+        <v>161.1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>181.65</v>
+      </c>
+      <c r="K15" s="3">
+        <v>214.76</v>
+      </c>
+      <c r="M15" s="1">
+        <v>11</v>
+      </c>
+      <c r="N15" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O15" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P15" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R15" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S15" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T15" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U15" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V15" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W15" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>69.7</v>
+      </c>
+      <c r="C16" s="2">
+        <v>80.53</v>
+      </c>
+      <c r="D16" s="2">
+        <v>91.35</v>
+      </c>
+      <c r="E16" s="2">
+        <v>101.42</v>
+      </c>
+      <c r="F16" s="2">
+        <v>111.48</v>
+      </c>
+      <c r="G16" s="2">
+        <v>121.55</v>
+      </c>
+      <c r="H16" s="2">
+        <v>142.29</v>
+      </c>
+      <c r="I16" s="2">
+        <v>163.02000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>183.76</v>
+      </c>
+      <c r="K16" s="3">
+        <v>215.81</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12</v>
+      </c>
+      <c r="N16" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O16" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P16" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R16" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S16" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T16" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U16" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V16" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W16" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="C17" s="2">
+        <v>82.24</v>
+      </c>
+      <c r="D17" s="2">
+        <v>93.43</v>
+      </c>
+      <c r="E17" s="2">
+        <v>103.32</v>
+      </c>
+      <c r="F17" s="2">
+        <v>113.21</v>
+      </c>
+      <c r="G17" s="2">
+        <v>123.09</v>
+      </c>
+      <c r="H17" s="2">
+        <v>144.02000000000001</v>
+      </c>
+      <c r="I17" s="2">
+        <v>164.94</v>
+      </c>
+      <c r="J17" s="2">
+        <v>185.86</v>
+      </c>
+      <c r="K17" s="3">
+        <v>216.86</v>
+      </c>
+      <c r="M17" s="1">
+        <v>13</v>
+      </c>
+      <c r="N17" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O17" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P17" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R17" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S17" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T17" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U17" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2">
+        <v>72.38</v>
+      </c>
+      <c r="C18" s="2">
+        <v>83.95</v>
+      </c>
+      <c r="D18" s="2">
+        <v>95.51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>105.22</v>
+      </c>
+      <c r="F18" s="2">
+        <v>114.93</v>
+      </c>
+      <c r="G18" s="2">
+        <v>124.63</v>
+      </c>
+      <c r="H18" s="2">
+        <v>145.75</v>
+      </c>
+      <c r="I18" s="2">
+        <v>166.86</v>
+      </c>
+      <c r="J18" s="2">
+        <v>187.97</v>
+      </c>
+      <c r="K18" s="3">
+        <v>217.92</v>
+      </c>
+      <c r="M18" s="1">
+        <v>14</v>
+      </c>
+      <c r="N18" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O18" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P18" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R18" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S18" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T18" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U18" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W18" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2">
+        <v>73.72</v>
+      </c>
+      <c r="C19" s="2">
+        <v>85.66</v>
+      </c>
+      <c r="D19" s="2">
+        <v>97.6</v>
+      </c>
+      <c r="E19" s="2">
+        <v>107.12</v>
+      </c>
+      <c r="F19" s="2">
+        <v>116.65</v>
+      </c>
+      <c r="G19" s="2">
+        <v>126.18</v>
+      </c>
+      <c r="H19" s="2">
+        <v>147.47999999999999</v>
+      </c>
+      <c r="I19" s="2">
+        <v>168.78</v>
+      </c>
+      <c r="J19" s="2">
+        <v>190.08</v>
+      </c>
+      <c r="K19" s="3">
+        <v>218.97</v>
+      </c>
+      <c r="M19" s="1">
+        <v>15</v>
+      </c>
+      <c r="N19" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O19" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P19" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R19" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S19" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T19" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U19" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V19" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W19" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2">
+        <v>75.05</v>
+      </c>
+      <c r="C20" s="2">
+        <v>87.37</v>
+      </c>
+      <c r="D20" s="2">
+        <v>99.68</v>
+      </c>
+      <c r="E20" s="2">
+        <v>109.02</v>
+      </c>
+      <c r="F20" s="2">
+        <v>118.37</v>
+      </c>
+      <c r="G20" s="2">
+        <v>127.72</v>
+      </c>
+      <c r="H20" s="2">
+        <v>149.21</v>
+      </c>
+      <c r="I20" s="2">
+        <v>170.69</v>
+      </c>
+      <c r="J20" s="2">
+        <v>192.18</v>
+      </c>
+      <c r="K20" s="3">
+        <v>220.02</v>
+      </c>
+      <c r="M20" s="1">
+        <v>16</v>
+      </c>
+      <c r="N20" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O20" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P20" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R20" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S20" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T20" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U20" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2">
+        <v>76.39</v>
+      </c>
+      <c r="C21" s="2">
+        <v>89.08</v>
+      </c>
+      <c r="D21" s="2">
+        <v>101.76</v>
+      </c>
+      <c r="E21" s="2">
+        <v>110.93</v>
+      </c>
+      <c r="F21" s="2">
+        <v>120.09</v>
+      </c>
+      <c r="G21" s="2">
+        <v>129.26</v>
+      </c>
+      <c r="H21" s="2">
+        <v>150.94</v>
+      </c>
+      <c r="I21" s="2">
+        <v>172.61</v>
+      </c>
+      <c r="J21" s="2">
+        <v>194.29</v>
+      </c>
+      <c r="K21" s="3">
+        <v>221.07</v>
+      </c>
+      <c r="M21" s="1">
+        <v>17</v>
+      </c>
+      <c r="N21" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O21" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P21" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R21" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S21" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T21" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U21" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V21" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W21" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2">
+        <v>77.73</v>
+      </c>
+      <c r="C22" s="2">
+        <v>90.79</v>
+      </c>
+      <c r="D22" s="2">
+        <v>103.84</v>
+      </c>
+      <c r="E22" s="2">
+        <v>112.83</v>
+      </c>
+      <c r="F22" s="2">
+        <v>121.81</v>
+      </c>
+      <c r="G22" s="2">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="H22" s="2">
+        <v>152.66</v>
+      </c>
+      <c r="I22" s="2">
+        <v>174.53</v>
+      </c>
+      <c r="J22" s="2">
+        <v>196.39</v>
+      </c>
+      <c r="K22" s="3">
+        <v>222.13</v>
+      </c>
+      <c r="M22" s="1">
+        <v>18</v>
+      </c>
+      <c r="N22" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O22" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P22" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R22" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S22" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T22" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U22" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V22" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W22" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2">
+        <v>79.069999999999993</v>
+      </c>
+      <c r="C23" s="2">
+        <v>92.5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>105.92</v>
+      </c>
+      <c r="E23" s="2">
+        <v>114.73</v>
+      </c>
+      <c r="F23" s="2">
+        <v>123.54</v>
+      </c>
+      <c r="G23" s="2">
+        <v>132.34</v>
+      </c>
+      <c r="H23" s="2">
+        <v>154.38999999999999</v>
+      </c>
+      <c r="I23" s="2">
+        <v>176.45</v>
+      </c>
+      <c r="J23" s="2">
+        <v>198.5</v>
+      </c>
+      <c r="K23" s="3">
+        <v>223.18</v>
+      </c>
+      <c r="M23" s="1">
+        <v>19</v>
+      </c>
+      <c r="N23" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O23" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P23" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R23" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S23" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T23" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U23" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V23" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W23" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2">
+        <v>80.41</v>
+      </c>
+      <c r="C24" s="2">
+        <v>94.21</v>
+      </c>
+      <c r="D24" s="2">
+        <v>108</v>
+      </c>
+      <c r="E24" s="2">
+        <v>116.63</v>
+      </c>
+      <c r="F24" s="2">
+        <v>125.26</v>
+      </c>
+      <c r="G24" s="2">
+        <v>133.88</v>
+      </c>
+      <c r="H24" s="2">
+        <v>156.12</v>
+      </c>
+      <c r="I24" s="2">
+        <v>178.36</v>
+      </c>
+      <c r="J24" s="2">
+        <v>200.6</v>
+      </c>
+      <c r="K24" s="3">
+        <v>224.23</v>
+      </c>
+      <c r="M24" s="1">
+        <v>20</v>
+      </c>
+      <c r="N24" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O24" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P24" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R24" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S24" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T24" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U24" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V24" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W24" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2">
+        <v>81.75</v>
+      </c>
+      <c r="C25" s="2">
+        <v>95.92</v>
+      </c>
+      <c r="D25" s="2">
+        <v>110.09</v>
+      </c>
+      <c r="E25" s="2">
+        <v>118.53</v>
+      </c>
+      <c r="F25" s="2">
+        <v>126.98</v>
+      </c>
+      <c r="G25" s="2">
+        <v>135.43</v>
+      </c>
+      <c r="H25" s="2">
+        <v>157.85</v>
+      </c>
+      <c r="I25" s="2">
+        <v>180.28</v>
+      </c>
+      <c r="J25" s="2">
+        <v>202.71</v>
+      </c>
+      <c r="K25" s="3">
+        <v>225.29</v>
+      </c>
+      <c r="M25" s="1">
+        <v>21</v>
+      </c>
+      <c r="N25" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O25" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P25" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R25" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S25" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T25" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U25" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V25" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W25" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2">
+        <v>83.08</v>
+      </c>
+      <c r="C26" s="2">
+        <v>97.63</v>
+      </c>
+      <c r="D26" s="2">
+        <v>112.17</v>
+      </c>
+      <c r="E26" s="2">
+        <v>120.43</v>
+      </c>
+      <c r="F26" s="2">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>136.97</v>
+      </c>
+      <c r="H26" s="2">
+        <v>159.58000000000001</v>
+      </c>
+      <c r="I26" s="2">
+        <v>182.2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>204.82</v>
+      </c>
+      <c r="K26" s="3">
+        <v>226.34</v>
+      </c>
+      <c r="M26" s="1">
+        <v>22</v>
+      </c>
+      <c r="N26" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O26" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P26" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R26" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S26" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T26" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U26" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V26" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W26" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2">
+        <v>84.42</v>
+      </c>
+      <c r="C27" s="2">
+        <v>99.34</v>
+      </c>
+      <c r="D27" s="2">
+        <v>114.25</v>
+      </c>
+      <c r="E27" s="2">
+        <v>122.34</v>
+      </c>
+      <c r="F27" s="2">
+        <v>130.41999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>138.51</v>
+      </c>
+      <c r="H27" s="2">
+        <v>161.31</v>
+      </c>
+      <c r="I27" s="2">
+        <v>184.12</v>
+      </c>
+      <c r="J27" s="2">
+        <v>206.92</v>
+      </c>
+      <c r="K27" s="3">
+        <v>227.39</v>
+      </c>
+      <c r="M27" s="1">
+        <v>23</v>
+      </c>
+      <c r="N27" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O27" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P27" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R27" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S27" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T27" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U27" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V27" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2">
+        <v>85.76</v>
+      </c>
+      <c r="C28" s="2">
+        <v>101.05</v>
+      </c>
+      <c r="D28" s="2">
+        <v>116.33</v>
+      </c>
+      <c r="E28" s="2">
+        <v>124.24</v>
+      </c>
+      <c r="F28" s="2">
+        <v>132.13999999999999</v>
+      </c>
+      <c r="G28" s="2">
+        <v>140.05000000000001</v>
+      </c>
+      <c r="H28" s="2">
+        <v>163.04</v>
+      </c>
+      <c r="I28" s="2">
+        <v>186.03</v>
+      </c>
+      <c r="J28" s="2">
+        <v>209.03</v>
+      </c>
+      <c r="K28" s="3">
+        <v>228.44</v>
+      </c>
+      <c r="M28" s="1">
+        <v>24</v>
+      </c>
+      <c r="N28" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O28" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P28" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R28" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S28" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T28" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U28" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V28" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2">
+        <v>87.1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>102.76</v>
+      </c>
+      <c r="D29" s="2">
+        <v>118.41</v>
+      </c>
+      <c r="E29" s="2">
+        <v>126.14</v>
+      </c>
+      <c r="F29" s="2">
+        <v>133.87</v>
+      </c>
+      <c r="G29" s="2">
+        <v>141.59</v>
+      </c>
+      <c r="H29" s="2">
+        <v>164.77</v>
+      </c>
+      <c r="I29" s="2">
+        <v>187.95</v>
+      </c>
+      <c r="J29" s="2">
+        <v>211.13</v>
+      </c>
+      <c r="K29" s="3">
+        <v>229.5</v>
+      </c>
+      <c r="M29" s="1">
+        <v>25</v>
+      </c>
+      <c r="N29" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O29" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P29" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R29" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S29" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T29" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U29" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V29" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W29" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2">
+        <v>88.44</v>
+      </c>
+      <c r="C30" s="2">
+        <v>104.47</v>
+      </c>
+      <c r="D30" s="2">
+        <v>120.49</v>
+      </c>
+      <c r="E30" s="2">
+        <v>128.04</v>
+      </c>
+      <c r="F30" s="2">
+        <v>135.59</v>
+      </c>
+      <c r="G30" s="2">
+        <v>143.13</v>
+      </c>
+      <c r="H30" s="2">
+        <v>166.5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>189.87</v>
+      </c>
+      <c r="J30" s="2">
+        <v>213.24</v>
+      </c>
+      <c r="K30" s="3">
+        <v>230.55</v>
+      </c>
+      <c r="M30" s="1">
+        <v>26</v>
+      </c>
+      <c r="N30" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O30" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P30" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R30" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S30" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T30" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U30" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V30" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2">
+        <v>89.77</v>
+      </c>
+      <c r="C31" s="2">
+        <v>106.18</v>
+      </c>
+      <c r="D31" s="2">
+        <v>122.58</v>
+      </c>
+      <c r="E31" s="2">
+        <v>129.94</v>
+      </c>
+      <c r="F31" s="2">
+        <v>137.31</v>
+      </c>
+      <c r="G31" s="2">
+        <v>144.68</v>
+      </c>
+      <c r="H31" s="2">
+        <v>168.23</v>
+      </c>
+      <c r="I31" s="2">
+        <v>191.79</v>
+      </c>
+      <c r="J31" s="2">
+        <v>215.34</v>
+      </c>
+      <c r="K31" s="3">
+        <v>231.6</v>
+      </c>
+      <c r="M31" s="1">
+        <v>27</v>
+      </c>
+      <c r="N31" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O31" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P31" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R31" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S31" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T31" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U31" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V31" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W31" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2">
+        <v>91.11</v>
+      </c>
+      <c r="C32" s="2">
+        <v>107.89</v>
+      </c>
+      <c r="D32" s="2">
+        <v>124.66</v>
+      </c>
+      <c r="E32" s="2">
+        <v>131.84</v>
+      </c>
+      <c r="F32" s="2">
+        <v>139.03</v>
+      </c>
+      <c r="G32" s="2">
+        <v>146.22</v>
+      </c>
+      <c r="H32" s="2">
+        <v>169.96</v>
+      </c>
+      <c r="I32" s="2">
+        <v>193.71</v>
+      </c>
+      <c r="J32" s="2">
+        <v>217.45</v>
+      </c>
+      <c r="K32" s="3">
+        <v>232.66</v>
+      </c>
+      <c r="M32" s="1">
+        <v>28</v>
+      </c>
+      <c r="N32" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O32" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P32" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R32" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S32" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T32" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U32" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V32" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W32" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2">
+        <v>92.45</v>
+      </c>
+      <c r="C33" s="2">
+        <v>109.6</v>
+      </c>
+      <c r="D33" s="2">
+        <v>126.74</v>
+      </c>
+      <c r="E33" s="2">
+        <v>133.75</v>
+      </c>
+      <c r="F33" s="2">
+        <v>140.75</v>
+      </c>
+      <c r="G33" s="2">
+        <v>147.76</v>
+      </c>
+      <c r="H33" s="2">
+        <v>171.69</v>
+      </c>
+      <c r="I33" s="2">
+        <v>195.62</v>
+      </c>
+      <c r="J33" s="2">
+        <v>219.56</v>
+      </c>
+      <c r="K33" s="3">
+        <v>233.71</v>
+      </c>
+      <c r="M33" s="1">
+        <v>29</v>
+      </c>
+      <c r="N33" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O33" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P33" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R33" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S33" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T33" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U33" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V33" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W33" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2">
+        <v>93.79</v>
+      </c>
+      <c r="C34" s="2">
+        <v>111.31</v>
+      </c>
+      <c r="D34" s="2">
+        <v>128.82</v>
+      </c>
+      <c r="E34" s="2">
+        <v>135.65</v>
+      </c>
+      <c r="F34" s="2">
+        <v>142.47</v>
+      </c>
+      <c r="G34" s="2">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="H34" s="2">
+        <v>173.42</v>
+      </c>
+      <c r="I34" s="2">
+        <v>197.54</v>
+      </c>
+      <c r="J34" s="2">
+        <v>221.66</v>
+      </c>
+      <c r="K34" s="3">
+        <v>234.76</v>
+      </c>
+      <c r="M34" s="1">
+        <v>30</v>
+      </c>
+      <c r="N34" s="3">
+        <v>247.86</v>
+      </c>
+      <c r="O34" s="3">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P34" s="3">
+        <v>358.94</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>414.48</v>
+      </c>
+      <c r="R34" s="3">
+        <v>470.02</v>
+      </c>
+      <c r="S34" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T34" s="3">
+        <v>795.8</v>
+      </c>
+      <c r="U34" s="3">
+        <v>958.69</v>
+      </c>
+      <c r="V34" s="3">
+        <v>1121.58</v>
+      </c>
+      <c r="W34" s="3">
+        <v>1284.47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2">
+        <v>69.243999999999986</v>
+      </c>
+      <c r="C35" s="2">
+        <v>81.830333333333314</v>
+      </c>
+      <c r="D35" s="2">
+        <v>94.409666666666652</v>
+      </c>
+      <c r="E35" s="2">
+        <v>103.26933333333334</v>
+      </c>
+      <c r="F35" s="2">
+        <v>112.12766666666667</v>
+      </c>
+      <c r="G35" s="2">
+        <v>120.98733333333332</v>
+      </c>
+      <c r="H35" s="2">
+        <v>141.94966666666662</v>
+      </c>
+      <c r="I35" s="2">
+        <v>162.91166666666669</v>
+      </c>
+      <c r="J35" s="2">
+        <v>183.87566666666666</v>
+      </c>
+      <c r="K35" s="2">
+        <v>215.86866666666668</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="3">
+        <v>247.85999999999993</v>
+      </c>
+      <c r="O35" s="3">
+        <v>303.39999999999981</v>
+      </c>
+      <c r="P35" s="3">
+        <v>358.93999999999994</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>414.47999999999973</v>
+      </c>
+      <c r="R35" s="3">
+        <v>470.02000000000032</v>
+      </c>
+      <c r="S35" s="3">
+        <v>632.91</v>
+      </c>
+      <c r="T35" s="3">
+        <v>795.79999999999961</v>
+      </c>
+      <c r="U35" s="3">
+        <v>958.68999999999971</v>
+      </c>
+      <c r="V35" s="3">
+        <v>1121.5800000000008</v>
+      </c>
+      <c r="W35" s="3">
+        <v>1284.4700000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="N2:W2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D1968-5793-4D21-B24C-89D80D0D7CAC}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
@@ -696,7 +3030,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -728,7 +3062,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -796,7 +3130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -864,7 +3198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -932,7 +3266,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1000,7 +3334,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1068,7 +3402,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1136,7 +3470,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1204,7 +3538,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1272,7 +3606,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1340,7 +3674,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1408,7 +3742,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1476,7 +3810,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1544,7 +3878,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1612,7 +3946,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1680,7 +4014,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1748,7 +4082,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1816,7 +4150,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1884,7 +4218,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1952,7 +4286,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2020,7 +4354,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -2088,7 +4422,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2156,7 +4490,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2224,7 +4558,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2292,7 +4626,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2360,7 +4694,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2428,7 +4762,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2496,7 +4830,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2564,7 +4898,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -2632,7 +4966,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -2700,7 +5034,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -2768,7 +5102,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -2836,7 +5170,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -2904,7 +5238,7 @@
         <v>1289.25</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -2981,20 +5315,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3790BBC8-1243-4A56-B780-75692A787EEC}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -3022,7 +5356,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3054,7 +5388,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3122,7 +5456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -3190,7 +5524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3258,7 +5592,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3326,7 +5660,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3394,7 +5728,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -3462,7 +5796,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -3530,7 +5864,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -3598,7 +5932,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -3666,7 +6000,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -3734,7 +6068,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -3802,7 +6136,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -3870,7 +6204,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -3938,7 +6272,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -4006,7 +6340,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -4074,7 +6408,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -4142,7 +6476,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -4210,7 +6544,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -4278,7 +6612,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -4346,7 +6680,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -4414,7 +6748,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -4482,7 +6816,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -4550,7 +6884,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -4618,7 +6952,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -4686,7 +7020,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -4754,7 +7088,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -4822,7 +7156,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -4890,7 +7224,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -4958,7 +7292,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -5026,7 +7360,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -5094,7 +7428,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -5162,7 +7496,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -5230,7 +7564,7 @@
         <v>1297.53</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -5307,20 +7641,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FD970D-7BFD-41BD-A958-70C0FE799EAC}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -5348,7 +7682,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -5380,7 +7714,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -5448,7 +7782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -5516,7 +7850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -5584,7 +7918,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -5652,7 +7986,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -5720,7 +8054,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -5788,7 +8122,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -5856,7 +8190,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -5924,7 +8258,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -5992,7 +8326,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -6060,7 +8394,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -6128,7 +8462,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -6196,7 +8530,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -6264,7 +8598,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -6332,7 +8666,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -6400,7 +8734,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -6468,7 +8802,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -6536,7 +8870,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -6604,7 +8938,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -6672,7 +9006,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -6740,7 +9074,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -6808,7 +9142,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -6876,7 +9210,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -6944,7 +9278,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -7012,7 +9346,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -7080,7 +9414,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -7148,7 +9482,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -7216,7 +9550,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -7284,7 +9618,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -7352,7 +9686,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -7420,7 +9754,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -7488,7 +9822,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -7556,7 +9890,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -7633,20 +9967,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91798AA-0655-457F-85E2-BCBDCB548CAE}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -7674,7 +10008,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7706,7 +10040,7 @@
       <c r="V2" s="12"/>
       <c r="W2" s="12"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -7774,7 +10108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -7842,7 +10176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -7910,7 +10244,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -7978,7 +10312,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -8046,7 +10380,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -8114,7 +10448,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -8182,7 +10516,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -8250,7 +10584,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -8318,7 +10652,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -8386,7 +10720,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -8454,7 +10788,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -8522,7 +10856,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -8590,7 +10924,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -8658,7 +10992,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -8726,7 +11060,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -8794,7 +11128,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -8862,7 +11196,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -8930,7 +11264,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -8998,7 +11332,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -9066,7 +11400,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -9134,7 +11468,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -9202,7 +11536,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -9270,7 +11604,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -9338,7 +11672,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -9406,7 +11740,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -9474,7 +11808,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -9542,7 +11876,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -9610,7 +11944,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -9678,7 +12012,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -9746,7 +12080,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -9814,7 +12148,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -9882,7 +12216,7 @@
         <v>1303.01</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -9959,7 +12293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFFF00"/>
@@ -9968,7 +12302,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>